<commit_message>
excel corrected (outlier removed)
</commit_message>
<xml_diff>
--- a/data/heart_disease.xlsx
+++ b/data/heart_disease.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7A1C37D-8B15-7A43-A184-A04E245C4C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4F502093-4F66-B142-8738-A60AC5E93962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1400" windowWidth="23680" windowHeight="18380"/>
+    <workbookView xWindow="10240" yWindow="4360" windowWidth="23680" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="processed.cleveland" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -919,11 +919,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N304"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,43 +977,43 @@
         <v>63</v>
       </c>
       <c r="B2">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>63</v>
+        <v>145</v>
       </c>
       <c r="E2">
-        <v>63</v>
+        <v>233</v>
       </c>
       <c r="F2">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>63</v>
+        <v>150</v>
       </c>
       <c r="I2">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>63</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K2">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="L2">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="N2">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>